<commit_message>
calcolo del tempo per ciascuna fase, calcolo cluster corretti
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Numero elementi estratti</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Media elementi per cluster</t>
   </si>
   <si>
-    <t>700 immagini (LCS e L1)</t>
-  </si>
-  <si>
     <t>Tempo di esecuzione (s)</t>
   </si>
   <si>
@@ -42,15 +39,6 @@
     <t>Precisione media (%)</t>
   </si>
   <si>
-    <t>Numero immagini</t>
-  </si>
-  <si>
-    <t>700 immagini (L1)</t>
-  </si>
-  <si>
-    <t>700 immagini (LCS)</t>
-  </si>
-  <si>
     <t>Numero di elementi stimato</t>
   </si>
   <si>
@@ -64,6 +52,30 @@
   </si>
   <si>
     <t>100 immagini (LCS e L1)</t>
+  </si>
+  <si>
+    <t>Numero scansioni</t>
+  </si>
+  <si>
+    <t>700 scansioni (LCS e L1)</t>
+  </si>
+  <si>
+    <t>700 scansioni (L1)</t>
+  </si>
+  <si>
+    <t>700 scansioni (LCS)</t>
+  </si>
+  <si>
+    <t>Tempo estrazione (s)</t>
+  </si>
+  <si>
+    <t>Tempo calcolo distanze (s)</t>
+  </si>
+  <si>
+    <t>Numero cluster corretti</t>
+  </si>
+  <si>
+    <t>Numero elementi corretti</t>
   </si>
 </sst>
 </file>
@@ -476,31 +488,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I31"/>
+  <dimension ref="A2:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="22.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="25.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="19.1640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="22.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="22.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="23.83203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.1640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="22" customHeight="1">
+    <row r="2" spans="1:13" ht="22" customHeight="1">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>0</v>
@@ -512,18 +530,30 @@
         <v>2</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="19" customHeight="1">
+    </row>
+    <row r="3" spans="1:13" ht="19" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1">
         <v>700</v>
@@ -542,19 +572,23 @@
         <f>D3/E3</f>
         <v>6.7058388765705841</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4">
         <v>91303.5</v>
       </c>
-      <c r="H3" s="4">
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4">
         <v>87.56</v>
       </c>
-      <c r="I3" s="4">
-        <v>75.44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="19" customHeight="1">
+      <c r="M3" s="4">
+        <v>76.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="19" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1">
         <v>700</v>
@@ -573,19 +607,23 @@
         <f t="shared" ref="F4:F19" si="1">D4/E4</f>
         <v>8.3086080586080584</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4">
         <v>23761.3</v>
       </c>
-      <c r="H4" s="4">
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4">
         <v>84.17</v>
       </c>
-      <c r="I4" s="4">
+      <c r="M4" s="4">
         <v>68.53</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="19" customHeight="1">
+    <row r="5" spans="1:13" ht="19" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1">
         <v>700</v>
@@ -604,19 +642,23 @@
         <f t="shared" si="1"/>
         <v>6.8398039954768191</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4">
         <v>84992.5</v>
       </c>
-      <c r="H5" s="4">
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4">
         <v>88.05</v>
       </c>
-      <c r="I5" s="4">
+      <c r="M5" s="4">
         <v>73.47</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="19" customHeight="1">
+    <row r="6" spans="1:13" ht="19" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1">
         <v>200</v>
@@ -635,19 +677,23 @@
         <f t="shared" si="1"/>
         <v>18.703703703703702</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4">
         <v>6120.27</v>
       </c>
-      <c r="H6" s="4">
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4">
         <v>74.08</v>
       </c>
-      <c r="I6" s="4">
+      <c r="M6" s="4">
         <v>70.48</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="19" customHeight="1">
+    <row r="7" spans="1:13" ht="19" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1">
         <v>200</v>
@@ -666,19 +712,23 @@
         <f t="shared" si="1"/>
         <v>18.703703703703702</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4">
         <v>6440.03</v>
       </c>
-      <c r="H7" s="4">
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4">
         <v>73.790000000000006</v>
       </c>
-      <c r="I7" s="4">
+      <c r="M7" s="4">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="19" customHeight="1">
+    <row r="8" spans="1:13" ht="19" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1">
         <v>100</v>
@@ -697,19 +747,23 @@
         <f t="shared" si="1"/>
         <v>17.028985507246375</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4">
         <v>1660.23</v>
       </c>
-      <c r="H8" s="4">
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4">
         <v>67.22</v>
       </c>
-      <c r="I8" s="4">
+      <c r="M8" s="4">
         <v>65.61</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="19" customHeight="1">
+    <row r="9" spans="1:13" ht="19" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1">
         <v>100</v>
@@ -728,17 +782,21 @@
         <f t="shared" si="1"/>
         <v>17.803030303030305</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4">
         <v>2326.5300000000002</v>
       </c>
-      <c r="H9" s="4">
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4">
         <v>67.150000000000006</v>
       </c>
-      <c r="I9" s="4">
+      <c r="M9" s="4">
         <v>65.36</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="19" customHeight="1">
+    <row r="10" spans="1:13" ht="19" customHeight="1">
       <c r="C10" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -752,8 +810,12 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" ht="19" customHeight="1">
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" ht="19" customHeight="1">
       <c r="C11" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -767,8 +829,12 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" ht="19" customHeight="1">
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" ht="19" customHeight="1">
       <c r="C12" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -782,8 +848,12 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" ht="19" customHeight="1">
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" ht="19" customHeight="1">
       <c r="C13" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -797,8 +867,12 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" ht="19" customHeight="1">
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+    </row>
+    <row r="14" spans="1:13" ht="19" customHeight="1">
       <c r="C14" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -812,8 +886,12 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" ht="19" customHeight="1">
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+    </row>
+    <row r="15" spans="1:13" ht="19" customHeight="1">
       <c r="C15" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -827,8 +905,12 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" ht="19" customHeight="1">
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+    </row>
+    <row r="16" spans="1:13" ht="19" customHeight="1">
       <c r="C16" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -842,8 +924,12 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
-    </row>
-    <row r="17" spans="3:9" ht="19" customHeight="1">
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+    </row>
+    <row r="17" spans="3:13" ht="19" customHeight="1">
       <c r="C17" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -857,8 +943,12 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
-    </row>
-    <row r="18" spans="3:9" ht="19" customHeight="1">
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+    </row>
+    <row r="18" spans="3:13" ht="19" customHeight="1">
       <c r="C18" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -872,8 +962,12 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
-    </row>
-    <row r="19" spans="3:9" ht="19" customHeight="1">
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+    </row>
+    <row r="19" spans="3:13" ht="19" customHeight="1">
       <c r="C19" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -887,8 +981,12 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
-    </row>
-    <row r="20" spans="3:9" ht="19" customHeight="1">
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+    </row>
+    <row r="20" spans="3:13" ht="19" customHeight="1">
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -896,8 +994,12 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
-    </row>
-    <row r="21" spans="3:9" ht="19" customHeight="1">
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+    </row>
+    <row r="21" spans="3:13" ht="19" customHeight="1">
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -905,8 +1007,12 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
-    </row>
-    <row r="22" spans="3:9" ht="19" customHeight="1">
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+    </row>
+    <row r="22" spans="3:13" ht="19" customHeight="1">
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -914,8 +1020,12 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
-    </row>
-    <row r="23" spans="3:9" ht="19" customHeight="1">
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+    </row>
+    <row r="23" spans="3:13" ht="19" customHeight="1">
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -923,8 +1033,12 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
-    </row>
-    <row r="24" spans="3:9">
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+    </row>
+    <row r="24" spans="3:13">
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -932,8 +1046,12 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
-    </row>
-    <row r="25" spans="3:9">
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+    </row>
+    <row r="25" spans="3:13">
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -941,8 +1059,12 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
-    </row>
-    <row r="26" spans="3:9">
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+    </row>
+    <row r="26" spans="3:13">
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -950,8 +1072,12 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
-    </row>
-    <row r="27" spans="3:9">
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+    </row>
+    <row r="27" spans="3:13">
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -959,8 +1085,12 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
-    </row>
-    <row r="28" spans="3:9">
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+    </row>
+    <row r="28" spans="3:13">
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -968,8 +1098,12 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
-    </row>
-    <row r="29" spans="3:9">
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+    </row>
+    <row r="29" spans="3:13">
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
@@ -977,8 +1111,12 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
-    </row>
-    <row r="30" spans="3:9">
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+    </row>
+    <row r="30" spans="3:13">
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
@@ -986,8 +1124,12 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
-    </row>
-    <row r="31" spans="3:9">
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+    </row>
+    <row r="31" spans="3:13">
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -995,6 +1137,10 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
vari fix relazione, aggiunte immagini features
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>Numero clusters</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Numero cluster corretti</t>
   </si>
   <si>
-    <t>Numero elementi corretti</t>
-  </si>
-  <si>
     <t>16 scansioni (LCS e L1)</t>
   </si>
   <si>
@@ -178,6 +175,12 @@
   </si>
   <si>
     <t>Tempo clustering (s)</t>
+  </si>
+  <si>
+    <t>Elementi corretti (%)</t>
+  </si>
+  <si>
+    <t>Elementi corretti</t>
   </si>
 </sst>
 </file>
@@ -638,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:Q31"/>
+  <dimension ref="A2:R31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -658,25 +661,26 @@
     <col min="10" max="10" width="19.6640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="23.33203125" style="1" customWidth="1"/>
     <col min="12" max="12" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.83203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.1640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="18.1640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="19.1640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" s="7" customFormat="1" ht="29" customHeight="1">
+    <row r="2" spans="1:18" s="7" customFormat="1" ht="29" customHeight="1">
       <c r="A2" s="6"/>
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>0</v>
@@ -685,13 +689,13 @@
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>2</v>
@@ -700,16 +704,19 @@
         <v>14</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="19" customHeight="1">
+    <row r="3" spans="1:18" ht="19" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -742,14 +749,15 @@
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
-      <c r="N3" s="5">
+      <c r="N3" s="4"/>
+      <c r="O3" s="5">
         <v>0.87560000000000004</v>
       </c>
-      <c r="O3" s="5">
+      <c r="P3" s="5">
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="19" customHeight="1">
+    <row r="4" spans="1:18" ht="19" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -782,14 +790,15 @@
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="5">
+      <c r="N4" s="4"/>
+      <c r="O4" s="5">
         <v>0.8417</v>
       </c>
-      <c r="O4" s="5">
+      <c r="P4" s="5">
         <v>0.68530000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="19" customHeight="1">
+    <row r="5" spans="1:18" ht="19" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -822,14 +831,15 @@
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="5">
+      <c r="N5" s="4"/>
+      <c r="O5" s="5">
         <v>88.05</v>
       </c>
-      <c r="O5" s="5">
+      <c r="P5" s="5">
         <v>73.47</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="19" customHeight="1">
+    <row r="6" spans="1:18" ht="19" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -862,14 +872,15 @@
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="5">
+      <c r="N6" s="4"/>
+      <c r="O6" s="5">
         <v>74.08</v>
       </c>
-      <c r="O6" s="5">
+      <c r="P6" s="5">
         <v>70.48</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="19" customHeight="1">
+    <row r="7" spans="1:18" ht="19" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -902,14 +913,15 @@
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
-      <c r="N7" s="5">
+      <c r="N7" s="4"/>
+      <c r="O7" s="5">
         <v>73.790000000000006</v>
       </c>
-      <c r="O7" s="5">
+      <c r="P7" s="5">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="19" customHeight="1">
+    <row r="8" spans="1:18" ht="19" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -942,14 +954,15 @@
       </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
-      <c r="N8" s="5">
+      <c r="N8" s="4"/>
+      <c r="O8" s="5">
         <v>67.22</v>
       </c>
-      <c r="O8" s="5">
+      <c r="P8" s="5">
         <v>65.61</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="19" customHeight="1">
+    <row r="9" spans="1:18" ht="19" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -982,16 +995,17 @@
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="4"/>
-      <c r="N9" s="5">
+      <c r="N9" s="4"/>
+      <c r="O9" s="5">
         <v>67.150000000000006</v>
       </c>
-      <c r="O9" s="5">
+      <c r="P9" s="5">
         <v>65.36</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="19" customHeight="1">
+    <row r="10" spans="1:18" ht="19" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1">
         <v>16</v>
@@ -1034,15 +1048,19 @@
         <v>45</v>
       </c>
       <c r="N10" s="5">
+        <f>M10/D10</f>
+        <v>8.1818181818181818E-2</v>
+      </c>
+      <c r="O10" s="5">
         <v>0.74370000000000003</v>
       </c>
-      <c r="O10" s="5">
+      <c r="P10" s="5">
         <v>0.62909999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="19" customHeight="1">
+    <row r="11" spans="1:18" ht="19" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1">
         <v>16</v>
@@ -1085,16 +1103,20 @@
         <v>44</v>
       </c>
       <c r="N11" s="5">
+        <f t="shared" ref="N11:N24" si="4">M11/D11</f>
+        <v>0.08</v>
+      </c>
+      <c r="O11" s="5">
         <v>0.76559999999999995</v>
       </c>
-      <c r="O11" s="5">
+      <c r="P11" s="5">
         <v>0.6</v>
       </c>
-      <c r="Q11" s="8"/>
-    </row>
-    <row r="12" spans="1:17" ht="19" customHeight="1">
+      <c r="R11" s="8"/>
+    </row>
+    <row r="12" spans="1:18" ht="19" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1">
         <v>16</v>
@@ -1137,15 +1159,19 @@
         <v>18</v>
       </c>
       <c r="N12" s="5">
+        <f t="shared" si="4"/>
+        <v>3.272727272727273E-2</v>
+      </c>
+      <c r="O12" s="5">
         <v>0.65059999999999996</v>
       </c>
-      <c r="O12" s="5">
+      <c r="P12" s="5">
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="19" customHeight="1">
+    <row r="13" spans="1:18" ht="19" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1">
         <v>32</v>
@@ -1188,15 +1214,19 @@
         <v>11</v>
       </c>
       <c r="N13" s="5">
+        <f t="shared" si="4"/>
+        <v>1.375E-2</v>
+      </c>
+      <c r="O13" s="5">
         <v>0.59850000000000003</v>
       </c>
-      <c r="O13" s="5">
+      <c r="P13" s="5">
         <v>0.52869999999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="19" customHeight="1">
+    <row r="14" spans="1:18" ht="19" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1">
         <v>32</v>
@@ -1239,15 +1269,19 @@
         <v>48</v>
       </c>
       <c r="N14" s="5">
+        <f t="shared" si="4"/>
+        <v>0.06</v>
+      </c>
+      <c r="O14" s="5">
         <v>0.72970000000000002</v>
       </c>
-      <c r="O14" s="5">
+      <c r="P14" s="5">
         <v>0.55500000000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="19" customHeight="1">
+    <row r="15" spans="1:18" ht="19" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1">
         <v>32</v>
@@ -1290,15 +1324,19 @@
         <v>43</v>
       </c>
       <c r="N15" s="5">
+        <f t="shared" si="4"/>
+        <v>5.3749999999999999E-2</v>
+      </c>
+      <c r="O15" s="5">
         <v>0.70189999999999997</v>
       </c>
-      <c r="O15" s="5">
+      <c r="P15" s="5">
         <v>0.5625</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="19" customHeight="1">
+    <row r="16" spans="1:18" ht="19" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1">
         <v>80</v>
@@ -1341,15 +1379,19 @@
         <v>316</v>
       </c>
       <c r="N16" s="5">
+        <f t="shared" si="4"/>
+        <v>0.13446808510638297</v>
+      </c>
+      <c r="O16" s="5">
         <v>0.78010000000000002</v>
       </c>
-      <c r="O16" s="5">
+      <c r="P16" s="5">
         <v>0.71160000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="19" customHeight="1">
+    <row r="17" spans="1:16" ht="19" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="1">
         <v>80</v>
@@ -1392,15 +1434,19 @@
         <v>265</v>
       </c>
       <c r="N17" s="5">
+        <f t="shared" si="4"/>
+        <v>0.11276595744680851</v>
+      </c>
+      <c r="O17" s="5">
         <v>0.75090000000000001</v>
       </c>
-      <c r="O17" s="5">
+      <c r="P17" s="5">
         <v>0.67490000000000006</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="19" customHeight="1">
+    <row r="18" spans="1:16" ht="19" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1">
         <v>80</v>
@@ -1443,21 +1489,25 @@
         <v>172</v>
       </c>
       <c r="N18" s="5">
+        <f t="shared" si="4"/>
+        <v>7.3191489361702125E-2</v>
+      </c>
+      <c r="O18" s="5">
         <v>0.69030000000000002</v>
       </c>
-      <c r="O18" s="5">
+      <c r="P18" s="5">
         <v>0.63649999999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="19" customHeight="1">
+    <row r="19" spans="1:16" ht="19" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="1">
         <v>160</v>
       </c>
       <c r="C19" s="4">
-        <f t="shared" ref="C19:C24" si="4">B19*50</f>
+        <f t="shared" ref="C19:C24" si="5">B19*50</f>
         <v>8000</v>
       </c>
       <c r="D19" s="4"/>
@@ -1479,18 +1529,22 @@
       <c r="K19" s="3"/>
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
-      <c r="N19" s="5"/>
+      <c r="N19" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="O19" s="5"/>
-    </row>
-    <row r="20" spans="1:15" ht="19" customHeight="1">
+      <c r="P19" s="5"/>
+    </row>
+    <row r="20" spans="1:16" ht="19" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="1">
         <v>160</v>
       </c>
       <c r="C20" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8000</v>
       </c>
       <c r="D20" s="3"/>
@@ -1512,18 +1566,22 @@
       <c r="K20" s="3"/>
       <c r="L20" s="4"/>
       <c r="M20" s="4"/>
-      <c r="N20" s="5"/>
+      <c r="N20" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="O20" s="5"/>
-    </row>
-    <row r="21" spans="1:15" ht="19" customHeight="1">
+      <c r="P20" s="5"/>
+    </row>
+    <row r="21" spans="1:16" ht="19" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="1">
         <v>160</v>
       </c>
       <c r="C21" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8000</v>
       </c>
       <c r="D21" s="3"/>
@@ -1545,10 +1603,14 @@
       <c r="K21" s="3"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
-      <c r="N21" s="5"/>
+      <c r="N21" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="O21" s="5"/>
-    </row>
-    <row r="22" spans="1:15" ht="19" customHeight="1">
+      <c r="P21" s="5"/>
+    </row>
+    <row r="22" spans="1:16" ht="19" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -1556,7 +1618,7 @@
         <v>700</v>
       </c>
       <c r="C22" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>35000</v>
       </c>
       <c r="D22" s="3"/>
@@ -1578,10 +1640,14 @@
       <c r="K22" s="3"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
-      <c r="N22" s="5"/>
+      <c r="N22" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="O22" s="5"/>
-    </row>
-    <row r="23" spans="1:15" ht="19" customHeight="1">
+      <c r="P22" s="5"/>
+    </row>
+    <row r="23" spans="1:16" ht="19" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
@@ -1589,7 +1655,7 @@
         <v>700</v>
       </c>
       <c r="C23" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>35000</v>
       </c>
       <c r="D23" s="3"/>
@@ -1611,10 +1677,14 @@
       <c r="K23" s="3"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
-      <c r="N23" s="5"/>
+      <c r="N23" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="O23" s="5"/>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="P23" s="5"/>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" s="1" t="s">
         <v>10</v>
       </c>
@@ -1622,7 +1692,7 @@
         <v>700</v>
       </c>
       <c r="C24" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>35000</v>
       </c>
       <c r="D24" s="3"/>
@@ -1644,10 +1714,14 @@
       <c r="K24" s="3"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
-      <c r="N24" s="5"/>
+      <c r="N24" s="5" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="O24" s="5"/>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="P24" s="5"/>
+    </row>
+    <row r="25" spans="1:16">
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -1661,8 +1735,9 @@
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="P25" s="3"/>
+    </row>
+    <row r="26" spans="1:16">
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -1676,8 +1751,9 @@
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="P26" s="3"/>
+    </row>
+    <row r="27" spans="1:16">
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -1691,8 +1767,9 @@
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="P27" s="3"/>
+    </row>
+    <row r="28" spans="1:16">
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -1706,8 +1783,9 @@
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="P28" s="3"/>
+    </row>
+    <row r="29" spans="1:16">
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -1721,8 +1799,9 @@
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="P29" s="3"/>
+    </row>
+    <row r="30" spans="1:16">
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -1736,8 +1815,9 @@
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="P30" s="3"/>
+    </row>
+    <row r="31" spans="1:16">
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -1751,6 +1831,7 @@
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
media elementi in cluster corretti
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Numero clusters</t>
   </si>
@@ -129,18 +129,6 @@
     <t>32 scansioni (LCS)</t>
   </si>
   <si>
-    <t>80 scansioni (LCS)</t>
-  </si>
-  <si>
-    <t>80 scansioni (L1)</t>
-  </si>
-  <si>
-    <t>160 scansioni (L1)</t>
-  </si>
-  <si>
-    <t>160 scansioni (LCS)</t>
-  </si>
-  <si>
     <t>Parole estratte (%)</t>
   </si>
   <si>
@@ -165,13 +153,28 @@
     <t>32 scansioni</t>
   </si>
   <si>
-    <t>80 scansioni</t>
-  </si>
-  <si>
-    <t>160 scansioni</t>
-  </si>
-  <si>
     <t>700 scansioni</t>
+  </si>
+  <si>
+    <t>75 scansioni</t>
+  </si>
+  <si>
+    <t>75 scansioni (LCS)</t>
+  </si>
+  <si>
+    <t>75 scansioni (L1)</t>
+  </si>
+  <si>
+    <t>130 scansioni (L1)</t>
+  </si>
+  <si>
+    <t>130 scansioni (LCS)</t>
+  </si>
+  <si>
+    <t>130 scansioni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Media elementi in cluster corretti </t>
   </si>
 </sst>
 </file>
@@ -268,8 +271,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -286,9 +295,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -298,30 +304,39 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="17">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -651,1039 +666,1110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R24"/>
+  <dimension ref="A2:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="25.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="24.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.33203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="20.83203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="18.1640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="19.1640625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="13.33203125" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="11" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="18.5" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="11" style="1" customWidth="1"/>
+    <col min="17" max="17" width="10.33203125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" s="7" customFormat="1" ht="29" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:19" s="9" customFormat="1" ht="36" customHeight="1">
+      <c r="A2" s="8"/>
+      <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="19" customHeight="1">
+      <c r="A3" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="19" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="B3" s="1">
         <v>16</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <f t="shared" ref="C3:C10" si="0">B3*50</f>
         <v>800</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>550</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <f t="shared" ref="E3:E17" si="1">(D3)/C3</f>
         <v>0.6875</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>66</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <f t="shared" ref="G3:G17" si="2">D3/F3</f>
         <v>8.3333333333333339</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>6.84</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="2">
         <v>37.72</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3" s="2">
         <f>K3-I3-H3</f>
         <v>2.8499999999999979</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3" s="2">
         <v>47.41</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="3">
         <v>25</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M3" s="3">
         <v>45</v>
       </c>
-      <c r="N3" s="5">
+      <c r="N3" s="2">
+        <f>M3/L3</f>
+        <v>1.8</v>
+      </c>
+      <c r="O3" s="4">
         <f>M3/D3</f>
         <v>8.1818181818181818E-2</v>
       </c>
-      <c r="O3" s="3">
+      <c r="P3" s="2">
         <v>74.37</v>
       </c>
-      <c r="P3" s="3">
+      <c r="Q3" s="2">
         <v>62.91</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="19" customHeight="1">
+    <row r="4" spans="1:19" ht="19" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1">
         <v>16</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <f t="shared" si="0"/>
         <v>800</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>550</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <f t="shared" si="1"/>
         <v>0.6875</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>71</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <f t="shared" si="2"/>
         <v>7.746478873239437</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>6.84</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <v>34.4</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="2">
         <f t="shared" ref="J4:J17" si="3">K4-I4-H4</f>
         <v>3.1500000000000021</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="2">
         <v>44.39</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="3">
         <v>33</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="3">
         <v>44</v>
       </c>
-      <c r="N4" s="5">
-        <f t="shared" ref="N4:N17" si="4">M4/D4</f>
+      <c r="N4" s="2">
+        <f t="shared" ref="N4:N17" si="4">M4/L4</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="O4" s="4">
+        <f t="shared" ref="O4:O17" si="5">M4/D4</f>
         <v>0.08</v>
       </c>
-      <c r="O4" s="3">
+      <c r="P4" s="2">
         <v>76.56</v>
       </c>
-      <c r="P4" s="3">
+      <c r="Q4" s="2">
         <v>60</v>
       </c>
-      <c r="R4" s="8"/>
-    </row>
-    <row r="5" spans="1:18" ht="19" customHeight="1">
+      <c r="S4" s="5"/>
+    </row>
+    <row r="5" spans="1:19" ht="19" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="1">
         <v>16</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <f t="shared" si="0"/>
         <v>800</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>550</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <f t="shared" si="1"/>
         <v>0.6875</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>55</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>6.81</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <v>5.0199999999999996</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="2">
         <f t="shared" si="3"/>
         <v>3.6900000000000004</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="2">
         <v>15.52</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="3">
         <v>12</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="3">
         <v>18</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="2">
         <f t="shared" si="4"/>
+        <v>1.5</v>
+      </c>
+      <c r="O5" s="4">
+        <f t="shared" si="5"/>
         <v>3.272727272727273E-2</v>
       </c>
-      <c r="O5" s="3">
+      <c r="P5" s="2">
         <v>65.06</v>
       </c>
-      <c r="P5" s="3">
+      <c r="Q5" s="2">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="19" customHeight="1">
+    <row r="6" spans="1:19" ht="19" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="1">
         <v>32</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>800</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>67</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <f t="shared" si="2"/>
         <v>11.940298507462687</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>11.54</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <v>7.22</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="2">
         <f t="shared" si="3"/>
         <v>19.82</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="2">
         <v>38.58</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="3">
         <v>11</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="3">
         <v>11</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="2">
         <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="O6" s="4">
+        <f t="shared" si="5"/>
         <v>1.375E-2</v>
       </c>
-      <c r="O6" s="3">
+      <c r="P6" s="2">
         <v>59.85</v>
       </c>
-      <c r="P6" s="3">
+      <c r="Q6" s="2">
         <v>52.87</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="19" customHeight="1">
+    <row r="7" spans="1:19" ht="19" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B7" s="1">
         <v>32</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>800</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>92</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <f t="shared" si="2"/>
         <v>8.695652173913043</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>11.27</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>74.72</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="2">
         <f t="shared" si="3"/>
         <v>8.5500000000000078</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="2">
         <v>94.54</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="3">
         <v>39</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="3">
         <v>48</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="2">
         <f t="shared" si="4"/>
+        <v>1.2307692307692308</v>
+      </c>
+      <c r="O7" s="4">
+        <f t="shared" si="5"/>
         <v>0.06</v>
       </c>
-      <c r="O7" s="3">
+      <c r="P7" s="2">
         <v>72.97</v>
       </c>
-      <c r="P7" s="3">
+      <c r="Q7" s="2">
         <v>55.5</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="19" customHeight="1">
+    <row r="8" spans="1:19" ht="19" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B8" s="1">
         <v>32</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>800</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>86</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <f t="shared" si="2"/>
         <v>9.3023255813953494</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>11.34</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <v>89.96</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="2">
         <f t="shared" si="3"/>
         <v>11.600000000000012</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="2">
         <v>112.9</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="3">
         <v>32</v>
       </c>
-      <c r="M8" s="4">
+      <c r="M8" s="3">
         <v>43</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="2">
         <f t="shared" si="4"/>
+        <v>1.34375</v>
+      </c>
+      <c r="O8" s="4">
+        <f t="shared" si="5"/>
         <v>5.3749999999999999E-2</v>
       </c>
-      <c r="O8" s="3">
+      <c r="P8" s="2">
         <v>70.19</v>
       </c>
-      <c r="P8" s="3">
+      <c r="Q8" s="2">
         <v>56.25</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="19" customHeight="1">
+    <row r="9" spans="1:19" ht="19" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1">
-        <v>80</v>
-      </c>
-      <c r="C9" s="4">
+        <v>75</v>
+      </c>
+      <c r="C9" s="3">
         <f t="shared" si="0"/>
-        <v>4000</v>
-      </c>
-      <c r="D9" s="4">
+        <v>3750</v>
+      </c>
+      <c r="D9" s="3">
         <v>2350</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <f t="shared" si="1"/>
-        <v>0.58750000000000002</v>
-      </c>
-      <c r="F9" s="4">
+        <v>0.62666666666666671</v>
+      </c>
+      <c r="F9" s="3">
         <v>199</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <f t="shared" si="2"/>
         <v>11.809045226130653</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>34.700000000000003</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <v>1070.92</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="2">
         <f t="shared" si="3"/>
         <v>97.659999999999897</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="2">
         <v>1203.28</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="3">
         <v>77</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M9" s="3">
         <v>316</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="2">
         <f t="shared" si="4"/>
+        <v>4.1038961038961039</v>
+      </c>
+      <c r="O9" s="4">
+        <f t="shared" si="5"/>
         <v>0.13446808510638297</v>
       </c>
-      <c r="O9" s="3">
+      <c r="P9" s="2">
         <v>78.010000000000005</v>
       </c>
-      <c r="P9" s="3">
+      <c r="Q9" s="2">
         <v>71.16</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="19" customHeight="1">
+    <row r="10" spans="1:19" ht="19" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1">
-        <v>80</v>
-      </c>
-      <c r="C10" s="4">
+        <v>75</v>
+      </c>
+      <c r="C10" s="3">
         <f t="shared" si="0"/>
-        <v>4000</v>
-      </c>
-      <c r="D10" s="4">
+        <v>3750</v>
+      </c>
+      <c r="D10" s="3">
         <v>2350</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <f t="shared" si="1"/>
-        <v>0.58750000000000002</v>
-      </c>
-      <c r="F10" s="4">
+        <v>0.62666666666666671</v>
+      </c>
+      <c r="F10" s="3">
         <v>189</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <f t="shared" si="2"/>
         <v>12.433862433862434</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <v>35.130000000000003</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="2">
         <v>1002.63</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="2">
         <f t="shared" si="3"/>
         <v>131.96000000000004</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="2">
         <v>1169.72</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="3">
         <v>78</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10" s="3">
         <v>265</v>
       </c>
-      <c r="N10" s="5">
+      <c r="N10" s="2">
         <f t="shared" si="4"/>
+        <v>3.3974358974358974</v>
+      </c>
+      <c r="O10" s="4">
+        <f t="shared" si="5"/>
         <v>0.11276595744680851</v>
       </c>
-      <c r="O10" s="3">
+      <c r="P10" s="2">
         <v>75.09</v>
       </c>
-      <c r="P10" s="3">
+      <c r="Q10" s="2">
         <v>67.489999999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="19" customHeight="1">
+    <row r="11" spans="1:19" ht="19" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1">
-        <v>80</v>
-      </c>
-      <c r="C11" s="4">
+        <v>75</v>
+      </c>
+      <c r="C11" s="3">
         <f>B11*50</f>
-        <v>4000</v>
-      </c>
-      <c r="D11" s="4">
+        <v>3750</v>
+      </c>
+      <c r="D11" s="3">
         <v>2350</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <f t="shared" si="1"/>
-        <v>0.58750000000000002</v>
-      </c>
-      <c r="F11" s="4">
+        <v>0.62666666666666671</v>
+      </c>
+      <c r="F11" s="3">
         <v>173</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <f>D11/F11</f>
         <v>13.583815028901734</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="2">
         <v>33.65</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="2">
         <v>69</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="2">
         <f t="shared" si="3"/>
         <v>118.38</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11" s="2">
         <v>221.03</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="3">
         <v>39</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11" s="3">
         <v>172</v>
       </c>
-      <c r="N11" s="5">
+      <c r="N11" s="2">
         <f t="shared" si="4"/>
+        <v>4.4102564102564106</v>
+      </c>
+      <c r="O11" s="4">
+        <f t="shared" si="5"/>
         <v>7.3191489361702125E-2</v>
       </c>
-      <c r="O11" s="3">
+      <c r="P11" s="2">
         <v>69.03</v>
       </c>
-      <c r="P11" s="3">
+      <c r="Q11" s="2">
         <v>63.65</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="19" customHeight="1">
+    <row r="12" spans="1:19" ht="19" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1">
-        <v>160</v>
-      </c>
-      <c r="C12" s="4">
-        <f t="shared" ref="C12:C17" si="5">B12*50</f>
-        <v>8000</v>
-      </c>
-      <c r="D12" s="4">
+        <v>130</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" ref="C12:C17" si="6">B12*50</f>
+        <v>6500</v>
+      </c>
+      <c r="D12" s="3">
         <v>5050</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <f t="shared" si="1"/>
-        <v>0.63124999999999998</v>
-      </c>
-      <c r="F12" s="4">
+        <v>0.77692307692307694</v>
+      </c>
+      <c r="F12" s="3">
         <v>425</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <f t="shared" si="2"/>
         <v>11.882352941176471</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <v>70.8</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="2">
         <v>313.7</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="2">
         <f t="shared" si="3"/>
         <v>5059.93</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="2">
         <v>5444.43</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12" s="3">
         <v>138</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12" s="3">
         <v>651</v>
       </c>
-      <c r="N12" s="5">
+      <c r="N12" s="2">
         <f t="shared" si="4"/>
+        <v>4.7173913043478262</v>
+      </c>
+      <c r="O12" s="4">
+        <f t="shared" si="5"/>
         <v>0.12891089108910891</v>
       </c>
-      <c r="O12" s="3">
+      <c r="P12" s="2">
         <v>76.66</v>
       </c>
-      <c r="P12" s="3">
+      <c r="Q12" s="2">
         <v>71.12</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="19" customHeight="1">
+    <row r="13" spans="1:19" ht="19" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1">
-        <v>160</v>
-      </c>
-      <c r="C13" s="4">
-        <f t="shared" si="5"/>
-        <v>8000</v>
-      </c>
-      <c r="D13" s="4">
+        <v>130</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="6"/>
+        <v>6500</v>
+      </c>
+      <c r="D13" s="3">
         <v>5050</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <f t="shared" si="1"/>
-        <v>0.63124999999999998</v>
-      </c>
-      <c r="F13" s="9">
+        <v>0.77692307692307694</v>
+      </c>
+      <c r="F13" s="6">
         <v>441</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="2">
         <f t="shared" si="2"/>
         <v>11.45124716553288</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="2">
         <v>68.171000000000006</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="2">
         <v>4353.8500000000004</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="2">
         <f t="shared" si="3"/>
         <v>1207.6889999999996</v>
       </c>
-      <c r="K13" s="3">
+      <c r="K13" s="2">
         <v>5629.71</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13" s="3">
         <v>208</v>
       </c>
-      <c r="M13" s="4">
+      <c r="M13" s="3">
         <v>713</v>
       </c>
-      <c r="N13" s="5">
+      <c r="N13" s="2">
         <f t="shared" si="4"/>
+        <v>3.4278846153846154</v>
+      </c>
+      <c r="O13" s="4">
+        <f t="shared" si="5"/>
         <v>0.14118811881188117</v>
       </c>
-      <c r="O13" s="3">
+      <c r="P13" s="2">
         <v>82.11</v>
       </c>
-      <c r="P13" s="3">
+      <c r="Q13" s="2">
         <v>74.41</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="19" customHeight="1">
+    <row r="14" spans="1:19" ht="19" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1">
-        <v>160</v>
-      </c>
-      <c r="C14" s="4">
-        <f t="shared" si="5"/>
-        <v>8000</v>
-      </c>
-      <c r="D14" s="4">
+        <v>130</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="6"/>
+        <v>6500</v>
+      </c>
+      <c r="D14" s="3">
         <v>5050</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <f t="shared" si="1"/>
-        <v>0.63124999999999998</v>
-      </c>
-      <c r="F14" s="9">
+        <v>0.77692307692307694</v>
+      </c>
+      <c r="F14" s="6">
         <v>463</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="2">
         <f t="shared" si="2"/>
         <v>10.907127429805616</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="2">
         <v>73.099999999999994</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="2">
         <v>5608.82</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="2">
         <f t="shared" si="3"/>
         <v>1047.7000000000003</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14" s="2">
         <v>6729.62</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="3">
         <v>215</v>
       </c>
-      <c r="M14" s="4">
+      <c r="M14" s="3">
         <v>860</v>
       </c>
-      <c r="N14" s="5">
+      <c r="N14" s="2">
         <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="O14" s="4">
+        <f t="shared" si="5"/>
         <v>0.17029702970297031</v>
       </c>
-      <c r="O14" s="3">
+      <c r="P14" s="2">
         <v>84.87</v>
       </c>
-      <c r="P14" s="3">
+      <c r="Q14" s="2">
         <v>77.94</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="19" customHeight="1">
+    <row r="15" spans="1:19" ht="19" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="1">
         <v>700</v>
       </c>
-      <c r="C15" s="4">
-        <f t="shared" si="5"/>
+      <c r="C15" s="3">
+        <f t="shared" si="6"/>
         <v>35000</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5">
+      <c r="D15" s="3"/>
+      <c r="E15" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="3" t="e">
+      <c r="F15" s="6"/>
+      <c r="G15" s="2" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3">
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K15" s="3"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="5" t="e">
+      <c r="K15" s="2"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="2" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O15" s="5"/>
-      <c r="P15" s="3"/>
-    </row>
-    <row r="16" spans="1:18" ht="19" customHeight="1">
+      <c r="O15" s="4" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="2"/>
+    </row>
+    <row r="16" spans="1:19" ht="19" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="1">
         <v>700</v>
       </c>
-      <c r="C16" s="4">
-        <f t="shared" si="5"/>
+      <c r="C16" s="3">
+        <f t="shared" si="6"/>
         <v>35000</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5">
+      <c r="D16" s="3"/>
+      <c r="E16" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="3" t="e">
+      <c r="F16" s="6"/>
+      <c r="G16" s="2" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3">
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K16" s="3"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="5" t="e">
+      <c r="K16" s="2"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="2" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O16" s="5"/>
-      <c r="P16" s="3"/>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="O16" s="4" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="2"/>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1">
         <v>700</v>
       </c>
-      <c r="C17" s="4">
-        <f t="shared" si="5"/>
+      <c r="C17" s="3">
+        <f t="shared" si="6"/>
         <v>35000</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="5">
+      <c r="D17" s="3"/>
+      <c r="E17" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="3" t="e">
+      <c r="F17" s="6"/>
+      <c r="G17" s="2" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="K17" s="3"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="5" t="e">
+      <c r="K17" s="2"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="2" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O17" s="5"/>
-      <c r="P17" s="3"/>
-    </row>
-    <row r="18" spans="1:16">
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-    </row>
-    <row r="19" spans="1:16">
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="O17" s="4" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="2"/>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="1">
         <v>700</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="3">
         <f>B20*50</f>
         <v>35000</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="3">
         <v>18146</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <f>(D20)/C20</f>
         <v>0.51845714285714284</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="3">
         <v>2706</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="2">
         <f>D20/F20</f>
         <v>6.7058388765705841</v>
       </c>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3">
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2">
         <v>91303.5</v>
       </c>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="5">
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="4">
         <v>0.87560000000000004</v>
       </c>
-      <c r="P20" s="3">
+      <c r="Q20" s="2">
         <v>0.76300000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:17">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="1">
         <v>700</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="3">
         <f>B21*50</f>
         <v>35000</v>
       </c>
-      <c r="D21" s="4">
+      <c r="D21" s="3">
         <v>18146</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="4">
         <f>(D21)/C21</f>
         <v>0.51845714285714284</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F21" s="3">
         <v>2184</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="2">
         <f>D21/F21</f>
         <v>8.3086080586080584</v>
       </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3">
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2">
         <v>23761.3</v>
       </c>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="5">
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="4">
         <v>0.8417</v>
       </c>
-      <c r="P21" s="3">
+      <c r="Q21" s="2">
         <v>0.68530000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:17">
       <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="1">
         <v>700</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C22" s="3">
         <f>B22*50</f>
         <v>35000</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D22" s="3">
         <v>18146</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="4">
         <f>(D22)/C22</f>
         <v>0.51845714285714284</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F22" s="3">
         <v>2653</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="2">
         <f>D22/F22</f>
         <v>6.8398039954768191</v>
       </c>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3">
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2">
         <v>84992.5</v>
       </c>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="5">
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="4">
         <v>0.88049999999999995</v>
       </c>
-      <c r="P22" s="3">
+      <c r="Q22" s="2">
         <v>0.73470000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-    </row>
-    <row r="24" spans="1:16">
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="3"/>
-      <c r="P24" s="3"/>
+    <row r="23" spans="1:17">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1704,51 +1790,51 @@
           <x14:sparklines>
             <x14:sparkline>
               <xm:f>Foglio1!A3:A3</xm:f>
-              <xm:sqref>P3</xm:sqref>
+              <xm:sqref>Q3</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Foglio1!A4:A4</xm:f>
-              <xm:sqref>P4</xm:sqref>
+              <xm:sqref>Q4</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Foglio1!A5:A5</xm:f>
-              <xm:sqref>P5</xm:sqref>
+              <xm:sqref>Q5</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Foglio1!A6:A6</xm:f>
-              <xm:sqref>P6</xm:sqref>
+              <xm:sqref>Q6</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Foglio1!A7:A7</xm:f>
-              <xm:sqref>P7</xm:sqref>
+              <xm:sqref>Q7</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Foglio1!A8:A8</xm:f>
-              <xm:sqref>P8</xm:sqref>
+              <xm:sqref>Q8</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Foglio1!A9:A9</xm:f>
-              <xm:sqref>P9</xm:sqref>
+              <xm:sqref>Q9</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Foglio1!A10:A10</xm:f>
-              <xm:sqref>P10</xm:sqref>
+              <xm:sqref>Q10</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Foglio1!A11:A11</xm:f>
-              <xm:sqref>P11</xm:sqref>
+              <xm:sqref>Q11</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Foglio1!A12:A12</xm:f>
-              <xm:sqref>P12</xm:sqref>
+              <xm:sqref>Q12</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Foglio1!A13:A13</xm:f>
-              <xm:sqref>P13</xm:sqref>
+              <xm:sqref>Q13</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Foglio1!A14:A14</xm:f>
-              <xm:sqref>P14</xm:sqref>
+              <xm:sqref>Q14</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>

</xml_diff>

<commit_message>
update risultati 500 immagini
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Numero clusters</t>
   </si>
@@ -99,9 +99,6 @@
     <t>Numero scansioni</t>
   </si>
   <si>
-    <t>700 scansioni (LCS e L1)</t>
-  </si>
-  <si>
     <t>700 scansioni (L1)</t>
   </si>
   <si>
@@ -147,18 +144,6 @@
     <t>Elementi corretti</t>
   </si>
   <si>
-    <t>16 scansioni</t>
-  </si>
-  <si>
-    <t>32 scansioni</t>
-  </si>
-  <si>
-    <t>700 scansioni</t>
-  </si>
-  <si>
-    <t>75 scansioni</t>
-  </si>
-  <si>
     <t>75 scansioni (LCS)</t>
   </si>
   <si>
@@ -171,10 +156,28 @@
     <t>130 scansioni (LCS)</t>
   </si>
   <si>
-    <t>130 scansioni</t>
-  </si>
-  <si>
     <t xml:space="preserve">Media elementi in cluster corretti </t>
+  </si>
+  <si>
+    <t>500 scansioni (L1)</t>
+  </si>
+  <si>
+    <t>500 scansioni (LCS)</t>
+  </si>
+  <si>
+    <t>16 scans</t>
+  </si>
+  <si>
+    <t>32 scans</t>
+  </si>
+  <si>
+    <t>75 scans</t>
+  </si>
+  <si>
+    <t>130 scans</t>
+  </si>
+  <si>
+    <t>500 scans</t>
   </si>
 </sst>
 </file>
@@ -271,8 +274,54 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -320,7 +369,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="63">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="5" builtinId="8" hidden="1"/>
@@ -329,6 +378,29 @@
     <cellStyle name="Collegamento ipertestuale" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="6" builtinId="9" hidden="1"/>
@@ -337,6 +409,29 @@
     <cellStyle name="Collegamento visitato" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -666,10 +761,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:S24"/>
+  <dimension ref="A2:S23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -700,13 +795,13 @@
         <v>5</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>0</v>
@@ -715,28 +810,28 @@
         <v>1</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P2" s="7" t="s">
         <v>4</v>
@@ -747,7 +842,7 @@
     </row>
     <row r="3" spans="1:19" ht="19" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1">
         <v>16</v>
@@ -806,7 +901,7 @@
     </row>
     <row r="4" spans="1:19" ht="19" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1">
         <v>16</v>
@@ -866,7 +961,7 @@
     </row>
     <row r="5" spans="1:19" ht="19" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1">
         <v>16</v>
@@ -925,7 +1020,7 @@
     </row>
     <row r="6" spans="1:19" ht="19" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1">
         <v>32</v>
@@ -984,7 +1079,7 @@
     </row>
     <row r="7" spans="1:19" ht="19" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1">
         <v>32</v>
@@ -1043,7 +1138,7 @@
     </row>
     <row r="8" spans="1:19" ht="19" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1">
         <v>32</v>
@@ -1102,7 +1197,7 @@
     </row>
     <row r="9" spans="1:19" ht="19" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B9" s="1">
         <v>75</v>
@@ -1161,7 +1256,7 @@
     </row>
     <row r="10" spans="1:19" ht="19" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1">
         <v>75</v>
@@ -1220,7 +1315,7 @@
     </row>
     <row r="11" spans="1:19" ht="19" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1">
         <v>75</v>
@@ -1279,7 +1374,7 @@
     </row>
     <row r="12" spans="1:19" ht="19" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1">
         <v>130</v>
@@ -1338,7 +1433,7 @@
     </row>
     <row r="13" spans="1:19" ht="19" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1">
         <v>130</v>
@@ -1397,7 +1492,7 @@
     </row>
     <row r="14" spans="1:19" ht="19" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14" s="1">
         <v>130</v>
@@ -1456,62 +1551,80 @@
     </row>
     <row r="15" spans="1:19" ht="19" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B15" s="1">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" si="6"/>
-        <v>35000</v>
-      </c>
-      <c r="D15" s="3"/>
+        <v>25000</v>
+      </c>
+      <c r="D15" s="3">
+        <v>18146</v>
+      </c>
       <c r="E15" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="2" t="e">
+        <v>0.72584000000000004</v>
+      </c>
+      <c r="F15" s="3">
+        <v>3941</v>
+      </c>
+      <c r="G15" s="2">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
+        <v>4.6044151230652117</v>
+      </c>
+      <c r="H15" s="2">
+        <v>403.41</v>
+      </c>
+      <c r="I15" s="2">
+        <v>61424.57</v>
+      </c>
       <c r="J15" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K15" s="2"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="2" t="e">
+        <v>76481.87</v>
+      </c>
+      <c r="K15" s="2">
+        <v>138309.85</v>
+      </c>
+      <c r="L15" s="3">
+        <v>3020</v>
+      </c>
+      <c r="M15" s="3">
+        <v>7616</v>
+      </c>
+      <c r="N15" s="2">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O15" s="4" t="e">
+        <v>2.5218543046357618</v>
+      </c>
+      <c r="O15" s="4">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="2"/>
+        <v>0.41970682244020718</v>
+      </c>
+      <c r="P15" s="2">
+        <v>92.27</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>82.14</v>
+      </c>
     </row>
     <row r="16" spans="1:19" ht="19" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" si="6"/>
-        <v>35000</v>
+        <v>25000</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F16" s="6"/>
+      <c r="F16" s="3"/>
       <c r="G16" s="2" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
@@ -1533,26 +1646,26 @@
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P16" s="4"/>
+      <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B17" s="1">
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="C17" s="3">
         <f t="shared" si="6"/>
-        <v>35000</v>
+        <v>25000</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F17" s="6"/>
+      <c r="F17" s="3"/>
       <c r="G17" s="2" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
@@ -1574,7 +1687,7 @@
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="P17" s="4"/>
+      <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
     <row r="18" spans="1:17">
@@ -1630,27 +1743,27 @@
         <v>0.51845714285714284</v>
       </c>
       <c r="F20" s="3">
-        <v>2706</v>
+        <v>2184</v>
       </c>
       <c r="G20" s="2">
         <f>D20/F20</f>
-        <v>6.7058388765705841</v>
+        <v>8.3086080586080584</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2">
-        <v>91303.5</v>
+        <v>23761.3</v>
       </c>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
       <c r="P20" s="4">
-        <v>0.87560000000000004</v>
+        <v>0.8417</v>
       </c>
       <c r="Q20" s="2">
-        <v>0.76300000000000001</v>
+        <v>0.68530000000000002</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1672,70 +1785,45 @@
         <v>0.51845714285714284</v>
       </c>
       <c r="F21" s="3">
-        <v>2184</v>
+        <v>2653</v>
       </c>
       <c r="G21" s="2">
         <f>D21/F21</f>
-        <v>8.3086080586080584</v>
+        <v>6.8398039954768191</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2">
-        <v>23761.3</v>
+        <v>84992.5</v>
       </c>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
       <c r="P21" s="4">
-        <v>0.8417</v>
+        <v>0.88049999999999995</v>
       </c>
       <c r="Q21" s="2">
-        <v>0.68530000000000002</v>
+        <v>0.73470000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:17">
-      <c r="A22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="1">
-        <v>700</v>
-      </c>
-      <c r="C22" s="3">
-        <f>B22*50</f>
-        <v>35000</v>
-      </c>
-      <c r="D22" s="3">
-        <v>18146</v>
-      </c>
-      <c r="E22" s="4">
-        <f>(D22)/C22</f>
-        <v>0.51845714285714284</v>
-      </c>
-      <c r="F22" s="3">
-        <v>2653</v>
-      </c>
-      <c r="G22" s="2">
-        <f>D22/F22</f>
-        <v>6.8398039954768191</v>
-      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-      <c r="K22" s="2">
-        <v>84992.5</v>
-      </c>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="4">
-        <v>0.88049999999999995</v>
-      </c>
-      <c r="Q22" s="2">
-        <v>0.73470000000000002</v>
-      </c>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
     </row>
     <row r="23" spans="1:17">
       <c r="C23" s="2"/>
@@ -1753,23 +1841,6 @@
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
-    </row>
-    <row r="24" spans="1:17">
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
risultati L1 500 immagini
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Numero clusters</t>
   </si>
@@ -97,12 +97,6 @@
   </si>
   <si>
     <t>Numero scansioni</t>
-  </si>
-  <si>
-    <t>700 scansioni (L1)</t>
-  </si>
-  <si>
-    <t>700 scansioni (LCS)</t>
   </si>
   <si>
     <t>Tempo calcolo distanze (s)</t>
@@ -274,8 +268,46 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -369,7 +401,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="101">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="5" builtinId="8" hidden="1"/>
@@ -401,6 +433,25 @@
     <cellStyle name="Collegamento ipertestuale" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="6" builtinId="9" hidden="1"/>
@@ -432,6 +483,25 @@
     <cellStyle name="Collegamento visitato" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -761,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:S23"/>
+  <dimension ref="A2:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -795,13 +865,13 @@
         <v>5</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>0</v>
@@ -810,28 +880,28 @@
         <v>1</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="P2" s="7" t="s">
         <v>4</v>
@@ -842,7 +912,7 @@
     </row>
     <row r="3" spans="1:19" ht="19" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3" s="1">
         <v>16</v>
@@ -901,7 +971,7 @@
     </row>
     <row r="4" spans="1:19" ht="19" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1">
         <v>16</v>
@@ -961,7 +1031,7 @@
     </row>
     <row r="5" spans="1:19" ht="19" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1">
         <v>16</v>
@@ -1020,7 +1090,7 @@
     </row>
     <row r="6" spans="1:19" ht="19" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1">
         <v>32</v>
@@ -1079,7 +1149,7 @@
     </row>
     <row r="7" spans="1:19" ht="19" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1">
         <v>32</v>
@@ -1138,7 +1208,7 @@
     </row>
     <row r="8" spans="1:19" ht="19" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1">
         <v>32</v>
@@ -1197,7 +1267,7 @@
     </row>
     <row r="9" spans="1:19" ht="19" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" s="1">
         <v>75</v>
@@ -1256,7 +1326,7 @@
     </row>
     <row r="10" spans="1:19" ht="19" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1">
         <v>75</v>
@@ -1315,7 +1385,7 @@
     </row>
     <row r="11" spans="1:19" ht="19" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1">
         <v>75</v>
@@ -1374,7 +1444,7 @@
     </row>
     <row r="12" spans="1:19" ht="19" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1">
         <v>130</v>
@@ -1433,7 +1503,7 @@
     </row>
     <row r="13" spans="1:19" ht="19" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1">
         <v>130</v>
@@ -1492,7 +1562,7 @@
     </row>
     <row r="14" spans="1:19" ht="19" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B14" s="1">
         <v>130</v>
@@ -1551,7 +1621,7 @@
     </row>
     <row r="15" spans="1:19" ht="19" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1">
         <v>500</v>
@@ -1610,7 +1680,7 @@
     </row>
     <row r="16" spans="1:19" ht="19" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B16" s="1">
         <v>500</v>
@@ -1651,7 +1721,7 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1">
         <v>500</v>
@@ -1660,35 +1730,53 @@
         <f t="shared" si="6"/>
         <v>25000</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="3">
+        <v>18146</v>
+      </c>
       <c r="E17" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="2" t="e">
+        <v>0.72584000000000004</v>
+      </c>
+      <c r="F17" s="3">
+        <v>3957</v>
+      </c>
+      <c r="G17" s="2">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+        <v>4.5857973212029313</v>
+      </c>
+      <c r="H17" s="2">
+        <v>289.33</v>
+      </c>
+      <c r="I17" s="2">
+        <v>4482.0200000000004</v>
+      </c>
       <c r="J17" s="2">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="K17" s="2"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="2" t="e">
+        <v>80773.759999999995</v>
+      </c>
+      <c r="K17" s="2">
+        <v>85545.11</v>
+      </c>
+      <c r="L17" s="3">
+        <v>2854</v>
+      </c>
+      <c r="M17" s="3">
+        <v>7354</v>
+      </c>
+      <c r="N17" s="2">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O17" s="4" t="e">
+        <v>2.5767344078486336</v>
+      </c>
+      <c r="O17" s="4">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
+        <v>0.40526837870605092</v>
+      </c>
+      <c r="P17" s="2">
+        <v>90.66</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>80.89</v>
+      </c>
     </row>
     <row r="18" spans="1:17">
       <c r="C18" s="2"/>
@@ -1725,122 +1813,38 @@
       <c r="Q19" s="2"/>
     </row>
     <row r="20" spans="1:17">
-      <c r="A20" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="1">
-        <v>700</v>
-      </c>
-      <c r="C20" s="3">
-        <f>B20*50</f>
-        <v>35000</v>
-      </c>
-      <c r="D20" s="3">
-        <v>18146</v>
-      </c>
-      <c r="E20" s="4">
-        <f>(D20)/C20</f>
-        <v>0.51845714285714284</v>
-      </c>
-      <c r="F20" s="3">
-        <v>2184</v>
-      </c>
-      <c r="G20" s="2">
-        <f>D20/F20</f>
-        <v>8.3086080586080584</v>
-      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="2">
-        <v>23761.3</v>
-      </c>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="3"/>
-      <c r="P20" s="4">
-        <v>0.8417</v>
-      </c>
-      <c r="Q20" s="2">
-        <v>0.68530000000000002</v>
-      </c>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
     </row>
     <row r="21" spans="1:17">
-      <c r="A21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="1">
-        <v>700</v>
-      </c>
-      <c r="C21" s="3">
-        <f>B21*50</f>
-        <v>35000</v>
-      </c>
-      <c r="D21" s="3">
-        <v>18146</v>
-      </c>
-      <c r="E21" s="4">
-        <f>(D21)/C21</f>
-        <v>0.51845714285714284</v>
-      </c>
-      <c r="F21" s="3">
-        <v>2653</v>
-      </c>
-      <c r="G21" s="2">
-        <f>D21/F21</f>
-        <v>6.8398039954768191</v>
-      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="2">
-        <v>84992.5</v>
-      </c>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="4">
-        <v>0.88049999999999995</v>
-      </c>
-      <c r="Q21" s="2">
-        <v>0.73470000000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17">
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
-    </row>
-    <row r="23" spans="1:17">
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
results and euclidean distance
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Numero clusters</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>500 scans</t>
+  </si>
+  <si>
+    <t>Cluster singoli</t>
   </si>
 </sst>
 </file>
@@ -959,35 +962,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:S21"/>
+  <dimension ref="A2:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5" style="1" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="14.6640625" style="1" customWidth="1"/>
     <col min="13" max="13" width="10.5" style="1" customWidth="1"/>
     <col min="14" max="14" width="18.5" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="11" style="1" customWidth="1"/>
-    <col min="17" max="17" width="10.33203125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="1"/>
+    <col min="15" max="16" width="12.33203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="11" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.33203125" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" s="9" customFormat="1" ht="36" customHeight="1">
+    <row r="2" spans="1:20" s="9" customFormat="1" ht="36" customHeight="1">
       <c r="A2" s="8"/>
       <c r="B2" s="7" t="s">
         <v>5</v>
@@ -1032,13 +1035,16 @@
         <v>17</v>
       </c>
       <c r="P2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="R2" s="7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="19" customHeight="1">
+    <row r="3" spans="1:20" ht="19" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
@@ -1090,14 +1096,17 @@
         <f>M3/D3</f>
         <v>8.1818181818181818E-2</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="3">
+        <v>18</v>
+      </c>
+      <c r="Q3" s="2">
         <v>74.37</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="R3" s="2">
         <v>62.91</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="19" customHeight="1">
+    <row r="4" spans="1:20" ht="19" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1149,15 +1158,18 @@
         <f t="shared" ref="O4:O17" si="5">M4/D4</f>
         <v>0.08</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="3">
+        <v>29</v>
+      </c>
+      <c r="Q4" s="2">
         <v>76.56</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="R4" s="2">
         <v>60</v>
       </c>
-      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
     </row>
-    <row r="5" spans="1:19" ht="19" customHeight="1">
+    <row r="5" spans="1:20" ht="19" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -1209,14 +1221,17 @@
         <f t="shared" si="5"/>
         <v>3.272727272727273E-2</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="3">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="2">
         <v>65.06</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="R5" s="2">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="19" customHeight="1">
+    <row r="6" spans="1:20" ht="19" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1268,14 +1283,17 @@
         <f t="shared" si="5"/>
         <v>1.375E-2</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="3">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="2">
         <v>59.85</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="R6" s="2">
         <v>52.87</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="19" customHeight="1">
+    <row r="7" spans="1:20" ht="19" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1327,14 +1345,17 @@
         <f t="shared" si="5"/>
         <v>0.06</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="3">
+        <v>36</v>
+      </c>
+      <c r="Q7" s="2">
         <v>72.97</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="R7" s="2">
         <v>55.5</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="19" customHeight="1">
+    <row r="8" spans="1:20" ht="19" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -1386,14 +1407,17 @@
         <f t="shared" si="5"/>
         <v>5.3749999999999999E-2</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8" s="3">
+        <v>28</v>
+      </c>
+      <c r="Q8" s="2">
         <v>70.19</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="R8" s="2">
         <v>56.25</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="19" customHeight="1">
+    <row r="9" spans="1:20" ht="19" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
@@ -1445,14 +1469,17 @@
         <f t="shared" si="5"/>
         <v>0.13446808510638297</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9" s="3">
+        <v>43</v>
+      </c>
+      <c r="Q9" s="2">
         <v>78.010000000000005</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="R9" s="2">
         <v>71.16</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="19" customHeight="1">
+    <row r="10" spans="1:20" ht="19" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -1504,14 +1531,17 @@
         <f t="shared" si="5"/>
         <v>0.11276595744680851</v>
       </c>
-      <c r="P10" s="2">
+      <c r="P10" s="3">
+        <v>43</v>
+      </c>
+      <c r="Q10" s="2">
         <v>75.09</v>
       </c>
-      <c r="Q10" s="2">
+      <c r="R10" s="2">
         <v>67.489999999999995</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="19" customHeight="1">
+    <row r="11" spans="1:20" ht="19" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -1563,14 +1593,17 @@
         <f t="shared" si="5"/>
         <v>7.3191489361702125E-2</v>
       </c>
-      <c r="P11" s="2">
+      <c r="P11" s="3">
+        <v>11</v>
+      </c>
+      <c r="Q11" s="2">
         <v>69.03</v>
       </c>
-      <c r="Q11" s="2">
+      <c r="R11" s="2">
         <v>63.65</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="19" customHeight="1">
+    <row r="12" spans="1:20" ht="19" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -1622,14 +1655,17 @@
         <f t="shared" si="5"/>
         <v>0.12891089108910891</v>
       </c>
-      <c r="P12" s="2">
+      <c r="P12" s="3">
+        <v>23</v>
+      </c>
+      <c r="Q12" s="2">
         <v>76.66</v>
       </c>
-      <c r="Q12" s="2">
+      <c r="R12" s="2">
         <v>71.12</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="19" customHeight="1">
+    <row r="13" spans="1:20" ht="19" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -1681,14 +1717,17 @@
         <f t="shared" si="5"/>
         <v>0.14118811881188117</v>
       </c>
-      <c r="P13" s="2">
+      <c r="P13" s="3">
+        <v>107</v>
+      </c>
+      <c r="Q13" s="2">
         <v>82.11</v>
       </c>
-      <c r="Q13" s="2">
+      <c r="R13" s="2">
         <v>74.41</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="19" customHeight="1">
+    <row r="14" spans="1:20" ht="19" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>29</v>
       </c>
@@ -1740,14 +1779,17 @@
         <f t="shared" si="5"/>
         <v>0.17029702970297031</v>
       </c>
-      <c r="P14" s="2">
+      <c r="P14" s="3">
+        <v>89</v>
+      </c>
+      <c r="Q14" s="2">
         <v>84.87</v>
       </c>
-      <c r="Q14" s="2">
+      <c r="R14" s="2">
         <v>77.94</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="19" customHeight="1">
+    <row r="15" spans="1:20" ht="19" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
@@ -1799,14 +1841,17 @@
         <f t="shared" si="5"/>
         <v>0.41970682244020718</v>
       </c>
-      <c r="P15" s="2">
+      <c r="P15" s="3">
+        <v>145</v>
+      </c>
+      <c r="Q15" s="2">
         <v>92.27</v>
       </c>
-      <c r="Q15" s="2">
+      <c r="R15" s="2">
         <v>82.14</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="19" customHeight="1">
+    <row r="16" spans="1:20" ht="19" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1858,14 +1903,17 @@
         <f t="shared" si="5"/>
         <v>0.40907086961313788</v>
       </c>
-      <c r="P16" s="2">
+      <c r="P16" s="3">
+        <v>163</v>
+      </c>
+      <c r="Q16" s="2">
         <v>91.02</v>
       </c>
-      <c r="Q16" s="2">
+      <c r="R16" s="2">
         <v>81.22</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:18">
       <c r="A17" s="1" t="s">
         <v>24</v>
       </c>
@@ -1917,14 +1965,17 @@
         <f t="shared" si="5"/>
         <v>0.40526837870605092</v>
       </c>
-      <c r="P17" s="2">
+      <c r="P17" s="3">
+        <v>151</v>
+      </c>
+      <c r="Q17" s="2">
         <v>90.66</v>
       </c>
-      <c r="Q17" s="2">
+      <c r="R17" s="2">
         <v>80.89</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:18">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1940,8 +1991,9 @@
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:18">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1957,8 +2009,9 @@
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:18">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1974,8 +2027,9 @@
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:18">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -1991,6 +2045,7 @@
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2011,51 +2066,51 @@
           <x14:sparklines>
             <x14:sparkline>
               <xm:f>Foglio1!A3:A3</xm:f>
-              <xm:sqref>Q3</xm:sqref>
+              <xm:sqref>R3</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Foglio1!A4:A4</xm:f>
-              <xm:sqref>Q4</xm:sqref>
+              <xm:sqref>R4</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Foglio1!A5:A5</xm:f>
-              <xm:sqref>Q5</xm:sqref>
+              <xm:sqref>R5</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Foglio1!A6:A6</xm:f>
-              <xm:sqref>Q6</xm:sqref>
+              <xm:sqref>R6</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Foglio1!A7:A7</xm:f>
-              <xm:sqref>Q7</xm:sqref>
+              <xm:sqref>R7</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Foglio1!A8:A8</xm:f>
-              <xm:sqref>Q8</xm:sqref>
+              <xm:sqref>R8</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Foglio1!A9:A9</xm:f>
-              <xm:sqref>Q9</xm:sqref>
+              <xm:sqref>R9</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Foglio1!A10:A10</xm:f>
-              <xm:sqref>Q10</xm:sqref>
+              <xm:sqref>R10</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Foglio1!A11:A11</xm:f>
-              <xm:sqref>Q11</xm:sqref>
+              <xm:sqref>R11</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Foglio1!A12:A12</xm:f>
-              <xm:sqref>Q12</xm:sqref>
+              <xm:sqref>R12</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Foglio1!A13:A13</xm:f>
-              <xm:sqref>Q13</xm:sqref>
+              <xm:sqref>R13</xm:sqref>
             </x14:sparkline>
             <x14:sparkline>
               <xm:f>Foglio1!A14:A14</xm:f>
-              <xm:sqref>Q14</xm:sqref>
+              <xm:sqref>R14</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>

</xml_diff>